<commit_message>
edit monopoly map, delete not unimplemented events
</commit_message>
<xml_diff>
--- a/Datas/MonopolyMap.xlsx
+++ b/Datas/MonopolyMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SunHeSLGConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8F5F95-CE83-4275-89A1-75AFF4202A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417C005A-BC77-4DED-A68F-C0A3EFC338A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="8100" windowWidth="24240" windowHeight="13140" xr2:uid="{120673EB-ED9A-45E0-B257-0DC0E06105DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{120673EB-ED9A-45E0-B257-0DC0E06105DF}"/>
   </bookViews>
   <sheets>
     <sheet name="MapConfig" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
   <si>
     <t>##var</t>
   </si>
@@ -222,9 +222,6 @@
     <t>bank heist</t>
   </si>
   <si>
-    <t>jail</t>
-  </si>
-  <si>
     <t>triggerOnPass</t>
   </si>
   <si>
@@ -240,43 +237,22 @@
     <t>string</t>
   </si>
   <si>
-    <t>COMMUNITY CHEST</t>
-  </si>
-  <si>
     <t>tileTitle</t>
   </si>
   <si>
-    <t>INCOME TAX</t>
-  </si>
-  <si>
-    <t>RAILROAD</t>
-  </si>
-  <si>
-    <t>AVENUE</t>
-  </si>
-  <si>
-    <t>CHANCE</t>
-  </si>
-  <si>
-    <t>JUST VISITING</t>
-  </si>
-  <si>
-    <t>ELECTRIC COMPANY</t>
-  </si>
-  <si>
-    <t>FREE PARKING</t>
-  </si>
-  <si>
-    <t>WATER WORKS</t>
-  </si>
-  <si>
-    <t>GO TO JAIL</t>
-  </si>
-  <si>
-    <t>LUXURY TAX</t>
-  </si>
-  <si>
-    <t>GO</t>
+    <t>Slot mini game</t>
+  </si>
+  <si>
+    <t>EARN</t>
+  </si>
+  <si>
+    <t>TAX</t>
+  </si>
+  <si>
+    <t>BANK</t>
+  </si>
+  <si>
+    <t>SLOT</t>
   </si>
 </sst>
 </file>
@@ -783,7 +759,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +784,7 @@
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
         <v>41</v>
@@ -820,7 +796,7 @@
         <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -841,13 +817,13 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -874,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -886,13 +862,13 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -910,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -958,13 +934,13 @@
       </c>
       <c r="E9" s="5"/>
       <c r="F9">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -976,13 +952,13 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -994,7 +970,7 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1018,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1032,11 +1008,14 @@
         <v>25</v>
       </c>
       <c r="E13" s="5"/>
+      <c r="F13">
+        <v>100</v>
+      </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1054,7 +1033,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1072,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1090,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -1102,13 +1081,13 @@
       </c>
       <c r="E17" s="5"/>
       <c r="F17">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -1138,13 +1117,13 @@
       </c>
       <c r="E19" s="5"/>
       <c r="F19">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -1156,13 +1135,13 @@
       </c>
       <c r="E20" s="5"/>
       <c r="F20">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -1174,7 +1153,7 @@
       </c>
       <c r="E21" s="5"/>
       <c r="F21">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1198,7 +1177,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -1212,11 +1191,14 @@
         <v>23</v>
       </c>
       <c r="E23" s="5"/>
+      <c r="F23">
+        <v>100</v>
+      </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1234,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -1246,13 +1228,13 @@
       </c>
       <c r="E25" s="5"/>
       <c r="F25">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -1270,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -1288,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -1318,13 +1300,13 @@
       </c>
       <c r="E29" s="5"/>
       <c r="F29">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -1336,13 +1318,13 @@
       </c>
       <c r="E30" s="5"/>
       <c r="F30">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
@@ -1360,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -1372,7 +1354,7 @@
       </c>
       <c r="E32" s="5"/>
       <c r="F32">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1393,13 +1375,13 @@
       </c>
       <c r="E33" s="5"/>
       <c r="F33">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -1417,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -1435,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
@@ -1453,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
@@ -1471,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
@@ -1501,13 +1483,13 @@
       </c>
       <c r="E39" s="5"/>
       <c r="F39">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
@@ -1519,13 +1501,13 @@
       </c>
       <c r="E40" s="5"/>
       <c r="F40">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
@@ -1537,13 +1519,13 @@
       </c>
       <c r="E41" s="5"/>
       <c r="F41">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -1561,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
@@ -1581,10 +1563,10 @@
         <v>100</v>
       </c>
       <c r="G43">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1598,7 +1580,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,7 +1626,7 @@
         <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1652,7 +1634,7 @@
         <v>101</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1668,7 +1650,7 @@
         <v>103</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add fishing mini game
</commit_message>
<xml_diff>
--- a/Datas/MonopolyMap.xlsx
+++ b/Datas/MonopolyMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SunHeSLGConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417C005A-BC77-4DED-A68F-C0A3EFC338A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859218F6-FF81-4504-9D11-A9E96D56A4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{120673EB-ED9A-45E0-B257-0DC0E06105DF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>##var</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>SLOT</t>
+  </si>
+  <si>
+    <t>Fishing mini game</t>
+  </si>
+  <si>
+    <t>FISH</t>
   </si>
 </sst>
 </file>
@@ -758,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9291EF3-8D1E-4249-88DF-DF32AB1F3002}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,13 +886,13 @@
       </c>
       <c r="E6" s="5"/>
       <c r="F6">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1027,13 +1033,13 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1192,13 +1198,13 @@
       </c>
       <c r="E23" s="5"/>
       <c r="F23">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1393,13 +1399,13 @@
       </c>
       <c r="E34" s="5"/>
       <c r="F34">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -1537,13 +1543,13 @@
       </c>
       <c r="E42" s="5"/>
       <c r="F42">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
@@ -1580,7 +1586,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,7 +1664,7 @@
         <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>